<commit_message>
[MDTUDDM-28147] Resource distribution for performance testing round.
Change-Id: Idd9a3682b78144e8c5fbbede24d17333010afaea
</commit_message>
<xml_diff>
--- a/docs/ua/modules/arch/attachments/architecture-workspace/performance/registry-resources.xlsx
+++ b/docs/ua/modules/arch/attachments/architecture-workspace/performance/registry-resources.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/docs/ua/modules/arch/attachments/architecture-workspace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/docs/ua/modules/arch/attachments/architecture-workspace/performance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C14BA1-830E-A849-9DAE-1CB3A87938DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E948735-BFDA-3048-BED2-06BF99938746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
   </bookViews>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C809D083-7CF6-1445-A306-E810BD791428}">
   <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V41" sqref="V41"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V39" sqref="V39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1375,7 +1375,7 @@
         <v>1000</v>
       </c>
       <c r="U6" s="6">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="V6" s="16" t="s">
         <v>128</v>
@@ -1693,10 +1693,10 @@
         <v>9</v>
       </c>
       <c r="T12" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="U12" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="V12" s="16" t="s">
         <v>128</v>
@@ -1865,10 +1865,10 @@
         <v>9</v>
       </c>
       <c r="T15" s="6">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="U15" s="6">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="V15" s="16" t="s">
         <v>128</v>
@@ -1929,10 +1929,10 @@
         <v>9</v>
       </c>
       <c r="T16" s="6">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="U16" s="6">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="V16" s="16" t="s">
         <v>128</v>
@@ -2223,10 +2223,10 @@
         <v>9</v>
       </c>
       <c r="T22" s="6">
+        <v>350</v>
+      </c>
+      <c r="U22" s="6">
         <v>400</v>
-      </c>
-      <c r="U22" s="6">
-        <v>500</v>
       </c>
       <c r="V22" s="16" t="s">
         <v>128</v>
@@ -2656,7 +2656,7 @@
         <v>400</v>
       </c>
       <c r="U29" s="6">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="V29" s="16" t="s">
         <v>128</v>
@@ -3109,10 +3109,10 @@
       <c r="R38" s="6"/>
       <c r="S38" s="4"/>
       <c r="T38" s="6">
+        <v>350</v>
+      </c>
+      <c r="U38" s="6">
         <v>400</v>
-      </c>
-      <c r="U38" s="6">
-        <v>500</v>
       </c>
       <c r="V38" s="16" t="s">
         <v>128</v>
@@ -3173,10 +3173,10 @@
         <v>9</v>
       </c>
       <c r="T39" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="U39" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="V39" s="16" t="s">
         <v>128</v>
@@ -3432,7 +3432,7 @@
         <v>400</v>
       </c>
       <c r="U43" s="6">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="V43" s="16" t="s">
         <v>128</v>
@@ -3496,7 +3496,7 @@
         <v>400</v>
       </c>
       <c r="U44" s="6">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="V44" s="16" t="s">
         <v>128</v>
@@ -3560,7 +3560,7 @@
         <v>400</v>
       </c>
       <c r="U45" s="6">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="V45" s="16" t="s">
         <v>128</v>
@@ -3624,7 +3624,7 @@
         <v>400</v>
       </c>
       <c r="U46" s="6">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="V46" s="16" t="s">
         <v>128</v>
@@ -3688,7 +3688,7 @@
         <v>400</v>
       </c>
       <c r="U47" s="6">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="V47" s="16" t="s">
         <v>128</v>
@@ -3816,7 +3816,7 @@
         <v>200</v>
       </c>
       <c r="U49" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="V49" s="16" t="s">
         <v>128</v>
@@ -3972,7 +3972,7 @@
         <v>400</v>
       </c>
       <c r="U52" s="6">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="V52" s="16" t="s">
         <v>128</v>
@@ -4036,7 +4036,7 @@
         <v>200</v>
       </c>
       <c r="U53" s="6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="V53" s="16" t="s">
         <v>128</v>
@@ -4238,7 +4238,7 @@
         <v>400</v>
       </c>
       <c r="U57" s="6">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="V57" s="16" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
[MDTUDDM-28147] - Resource distribution for performance testing round
Change-Id: Ib77af23b385c8d4de420f9f9903502eb1ac69e1b
</commit_message>
<xml_diff>
--- a/docs/ua/modules/arch/attachments/architecture-workspace/performance/registry-resources.xlsx
+++ b/docs/ua/modules/arch/attachments/architecture-workspace/performance/registry-resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/docs/ua/modules/arch/attachments/architecture-workspace/performance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yevhen_Zvarych\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E3BCA7-BD6D-F949-8BE4-66C59E660A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{27575FB0-79D4-4065-9287-79F5E4E42A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76BACE1B-BDCC-F34F-9205-7BB42BE8027F}"/>
   </bookViews>
   <sheets>
     <sheet name="Registry Resources" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="145">
   <si>
     <t>Technology</t>
   </si>
@@ -428,7 +428,49 @@
     <t>-XX:ActiveProcessorCount=2 -XX:+UseG1GC -XX:+ExplicitGCInvokesConcurrent</t>
   </si>
   <si>
+    <t>Istio sidecars</t>
+  </si>
+  <si>
+    <t>Container CPU requests</t>
+  </si>
+  <si>
+    <t>Container CPU limits</t>
+  </si>
+  <si>
+    <t>Container Memory requests</t>
+  </si>
+  <si>
+    <t>Container Memory Limits</t>
+  </si>
+  <si>
+    <t>2m</t>
+  </si>
+  <si>
+    <t>500m</t>
+  </si>
+  <si>
+    <t>60Mi</t>
+  </si>
+  <si>
+    <t>140Mi</t>
+  </si>
+  <si>
     <t>restic</t>
+  </si>
+  <si>
+    <t>50m</t>
+  </si>
+  <si>
+    <t>1500m</t>
+  </si>
+  <si>
+    <t>128Mi</t>
+  </si>
+  <si>
+    <t>1Gi</t>
+  </si>
+  <si>
+    <t>2000Mi</t>
   </si>
 </sst>
 </file>
@@ -619,7 +661,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="27">
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -703,40 +757,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}" name="Table3" displayName="Table3" ref="A1:V66" totalsRowShown="0" dataDxfId="22">
-  <autoFilter ref="A1:V66" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}">
-    <filterColumn colId="8">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}" name="Table3" displayName="Table3" ref="A1:Z67" totalsRowShown="0" dataDxfId="26">
+  <autoFilter ref="A1:Z67" xr:uid="{06C99DE8-B980-0548-85E0-AAF92621FDD9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:V58">
     <sortCondition ref="C1:C65"/>
   </sortState>
-  <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{7B40E2F0-02D6-904B-8018-66FABFA0DD1D}" name="Zone" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{9B6E3613-3147-0A49-A88D-DE5E5756377A}" name="Subsystem" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{7B693F86-BB20-4643-8C59-CE9AAFCBF004}" name="Component" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{BDC056D6-A828-3747-8D2F-B230006DB630}" name="Type" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{26E395E2-1F19-C84B-980C-08C4B5582553}" name="Deployment Mode" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{206BB385-4C22-624D-A2DB-36D434439669}" name="Min Profile" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{E36D12C6-BEC1-3841-BB7F-07B8DD85B728}" name="Service Mesh" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{DE3293B1-99DC-3448-B36C-7DC56C231CB7}" name="Monitoring" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{90E59384-34DA-9D4D-8715-BED9DC803BBE}" name="Technology" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{377A7AC7-A184-3C48-8086-D39E59847613}" name="CPU requests" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{A68A20D7-80D6-024B-9175-46DB49055D1E}" name="CPU limits" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{DEBD3593-F949-C44D-9F55-7F38F0A28A4E}" name="Memory requests" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{1196C492-F6F6-074A-B99F-1E8E358E5624}" name="Memory limits" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{7D3E02CE-7CDD-5E44-88DF-1162888AE695}" name="-Xms, Mb (baseline)" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{3D28B649-AB9D-9C49-8889-6B0D4888A8D3}" name="-Xmx, Mb (baseline)" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{729BA2AA-0236-6D4E-88FA-AF5279155852}" name="-Xmn, Mb (baseline)" dataDxfId="6"/>
-    <tableColumn id="22" xr3:uid="{4E8AEAD1-7BE7-C842-8ED6-80C30C596EB7}" name="Metaspace, Mb (baseline)" dataDxfId="5"/>
-    <tableColumn id="23" xr3:uid="{60B01E56-F1C6-2843-8907-B681700354AC}" name="GC (baseline)" dataDxfId="4"/>
-    <tableColumn id="24" xr3:uid="{48DAE9E5-2055-F847-BF1B-31D6835B4140}" name="Java Opts (baseline)" dataDxfId="3"/>
-    <tableColumn id="21" xr3:uid="{0E115C8F-10F3-1849-9086-23ECFF100762}" name="-Xms, Mb (target)" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{59ED4565-1835-554A-B6BE-EFEE9FF75498}" name="-Xmx, Mb (target)" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{8EF485D1-BA5B-0B42-B711-53E12FB7661E}" name="Java Opts (target)" dataDxfId="0"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{7B40E2F0-02D6-904B-8018-66FABFA0DD1D}" name="Zone" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{9B6E3613-3147-0A49-A88D-DE5E5756377A}" name="Subsystem" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{7B693F86-BB20-4643-8C59-CE9AAFCBF004}" name="Component" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{BDC056D6-A828-3747-8D2F-B230006DB630}" name="Type" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{26E395E2-1F19-C84B-980C-08C4B5582553}" name="Deployment Mode" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{206BB385-4C22-624D-A2DB-36D434439669}" name="Min Profile" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{E36D12C6-BEC1-3841-BB7F-07B8DD85B728}" name="Service Mesh" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{DE3293B1-99DC-3448-B36C-7DC56C231CB7}" name="Monitoring" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{90E59384-34DA-9D4D-8715-BED9DC803BBE}" name="Technology" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{377A7AC7-A184-3C48-8086-D39E59847613}" name="CPU requests" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{A68A20D7-80D6-024B-9175-46DB49055D1E}" name="CPU limits" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{DEBD3593-F949-C44D-9F55-7F38F0A28A4E}" name="Memory requests" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{1196C492-F6F6-074A-B99F-1E8E358E5624}" name="Memory limits" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{7D3E02CE-7CDD-5E44-88DF-1162888AE695}" name="-Xms, Mb (baseline)" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{3D28B649-AB9D-9C49-8889-6B0D4888A8D3}" name="-Xmx, Mb (baseline)" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{729BA2AA-0236-6D4E-88FA-AF5279155852}" name="-Xmn, Mb (baseline)" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{4E8AEAD1-7BE7-C842-8ED6-80C30C596EB7}" name="Metaspace, Mb (baseline)" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{60B01E56-F1C6-2843-8907-B681700354AC}" name="GC (baseline)" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{48DAE9E5-2055-F847-BF1B-31D6835B4140}" name="Java Opts (baseline)" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{0E115C8F-10F3-1849-9086-23ECFF100762}" name="-Xms, Mb (target)" dataDxfId="6"/>
+    <tableColumn id="20" xr3:uid="{59ED4565-1835-554A-B6BE-EFEE9FF75498}" name="-Xmx, Mb (target)" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{8EF485D1-BA5B-0B42-B711-53E12FB7661E}" name="Java Opts (target)" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{F8AE6B66-754A-4295-A46E-DC6FB4C9B908}" name="Container CPU requests" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{148AA45C-38C1-4AFE-8411-B1B3F9A43A7D}" name="Container CPU limits" dataDxfId="2"/>
+    <tableColumn id="25" xr3:uid="{834254E1-91DA-4CF3-A6CB-F499DF458075}" name="Container Memory requests" dataDxfId="1"/>
+    <tableColumn id="26" xr3:uid="{7FA4B471-0588-42B4-A76D-131846BA5700}" name="Container Memory Limits" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1039,39 +1091,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C809D083-7CF6-1445-A306-E810BD791428}">
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="65.83203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="28.796875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="65.796875" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="15.5" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.19921875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.296875" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="2" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.83203125" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.296875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.796875" style="2" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.69921875" style="2" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="2" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="21.296875" style="2" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="21.5" customWidth="1"/>
-    <col min="15" max="15" width="19.83203125" customWidth="1"/>
+    <col min="15" max="15" width="19.796875" customWidth="1"/>
     <col min="16" max="16" width="20.5" customWidth="1"/>
-    <col min="17" max="17" width="26.33203125" customWidth="1"/>
+    <col min="17" max="17" width="26.296875" customWidth="1"/>
     <col min="18" max="18" width="15.5" customWidth="1"/>
-    <col min="19" max="19" width="58.83203125" customWidth="1"/>
+    <col min="19" max="19" width="58.796875" customWidth="1"/>
     <col min="20" max="20" width="19.5" customWidth="1"/>
-    <col min="21" max="21" width="18.1640625" customWidth="1"/>
-    <col min="22" max="22" width="67.1640625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="18.19921875" customWidth="1"/>
+    <col min="22" max="22" width="67.19921875" style="3" customWidth="1"/>
+    <col min="23" max="23" width="23.5" customWidth="1"/>
+    <col min="24" max="24" width="20.5" customWidth="1"/>
+    <col min="25" max="25" width="27.09765625" customWidth="1"/>
+    <col min="26" max="26" width="25.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -1138,8 +1194,20 @@
       <c r="V1" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
@@ -1184,8 +1252,12 @@
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
-    </row>
-    <row r="3" spans="1:22" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+    </row>
+    <row r="3" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>72</v>
       </c>
@@ -1230,8 +1302,12 @@
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
-    </row>
-    <row r="4" spans="1:22" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+    </row>
+    <row r="4" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>72</v>
       </c>
@@ -1276,8 +1352,12 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
-    </row>
-    <row r="5" spans="1:22" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>72</v>
       </c>
@@ -1322,8 +1402,12 @@
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
-    </row>
-    <row r="6" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>73</v>
       </c>
@@ -1386,8 +1470,12 @@
       <c r="V6" s="16" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>72</v>
       </c>
@@ -1440,8 +1528,12 @@
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
-    </row>
-    <row r="8" spans="1:22" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
@@ -1486,8 +1578,12 @@
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
-    </row>
-    <row r="9" spans="1:22" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+    </row>
+    <row r="9" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>72</v>
       </c>
@@ -1532,8 +1628,12 @@
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
-    </row>
-    <row r="10" spans="1:22" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+    </row>
+    <row r="10" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>72</v>
       </c>
@@ -1578,8 +1678,12 @@
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
-    </row>
-    <row r="11" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="1:26" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>73</v>
       </c>
@@ -1643,8 +1747,12 @@
       <c r="V11" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>72</v>
       </c>
@@ -1707,8 +1815,12 @@
       <c r="V12" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>72</v>
       </c>
@@ -1759,10 +1871,18 @@
       <c r="R13" s="6"/>
       <c r="S13" s="4"/>
       <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
+      <c r="U13" s="6">
+        <v>1024</v>
+      </c>
       <c r="V13" s="6"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>72</v>
       </c>
@@ -1815,8 +1935,12 @@
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>72</v>
       </c>
@@ -1879,8 +2003,12 @@
       <c r="V15" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>73</v>
       </c>
@@ -1943,8 +2071,12 @@
       <c r="V16" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>72</v>
       </c>
@@ -1989,8 +2121,12 @@
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
-    </row>
-    <row r="18" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>73</v>
       </c>
@@ -2035,8 +2171,12 @@
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
-    </row>
-    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>73</v>
       </c>
@@ -2081,8 +2221,12 @@
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
-    </row>
-    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>73</v>
       </c>
@@ -2127,8 +2271,12 @@
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
-    </row>
-    <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>73</v>
       </c>
@@ -2173,8 +2321,12 @@
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>73</v>
       </c>
@@ -2237,8 +2389,12 @@
       <c r="V22" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>73</v>
       </c>
@@ -2301,8 +2457,12 @@
       <c r="V23" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>73</v>
       </c>
@@ -2365,8 +2525,12 @@
       <c r="V24" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+    </row>
+    <row r="25" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>73</v>
       </c>
@@ -2411,8 +2575,12 @@
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>73</v>
       </c>
@@ -2475,8 +2643,12 @@
       <c r="V26" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>73</v>
       </c>
@@ -2539,8 +2711,12 @@
       <c r="V27" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>73</v>
       </c>
@@ -2603,8 +2779,12 @@
       <c r="V28" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>73</v>
       </c>
@@ -2667,8 +2847,12 @@
       <c r="V29" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>73</v>
       </c>
@@ -2723,14 +2907,20 @@
         <v>9</v>
       </c>
       <c r="T30" s="6">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="U30" s="6">
         <v>500</v>
       </c>
-      <c r="V30" s="16"/>
-    </row>
-    <row r="31" spans="1:22" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V30" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+    </row>
+    <row r="31" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>73</v>
       </c>
@@ -2791,8 +2981,12 @@
       <c r="V31" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
@@ -2837,8 +3031,12 @@
       <c r="T32" s="6"/>
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
-    </row>
-    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W32" s="6"/>
+      <c r="X32" s="6"/>
+      <c r="Y32" s="6"/>
+      <c r="Z32" s="6"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>73</v>
       </c>
@@ -2883,8 +3081,12 @@
       <c r="T33" s="6"/>
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
-    </row>
-    <row r="34" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+      <c r="Y33" s="6"/>
+      <c r="Z33" s="6"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>73</v>
       </c>
@@ -2929,8 +3131,12 @@
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
-    </row>
-    <row r="35" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>73</v>
       </c>
@@ -2975,8 +3181,12 @@
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
-    </row>
-    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W35" s="6"/>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="6"/>
+      <c r="Z35" s="6"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>73</v>
       </c>
@@ -3021,8 +3231,12 @@
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
-    </row>
-    <row r="37" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W36" s="6"/>
+      <c r="X36" s="6"/>
+      <c r="Y36" s="6"/>
+      <c r="Z36" s="6"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>73</v>
       </c>
@@ -3067,8 +3281,12 @@
       <c r="T37" s="6"/>
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W37" s="6"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="6"/>
+      <c r="Z37" s="6"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>73</v>
       </c>
@@ -3127,8 +3345,12 @@
       <c r="V38" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W38" s="6"/>
+      <c r="X38" s="6"/>
+      <c r="Y38" s="6"/>
+      <c r="Z38" s="6"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>72</v>
       </c>
@@ -3191,8 +3413,12 @@
       <c r="V39" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
+      <c r="Y39" s="6"/>
+      <c r="Z39" s="6"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>73</v>
       </c>
@@ -3255,8 +3481,12 @@
       <c r="V40" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W40" s="6"/>
+      <c r="X40" s="6"/>
+      <c r="Y40" s="6"/>
+      <c r="Z40" s="6"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>73</v>
       </c>
@@ -3319,8 +3549,12 @@
       <c r="V41" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W41" s="6"/>
+      <c r="X41" s="6"/>
+      <c r="Y41" s="6"/>
+      <c r="Z41" s="6"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>73</v>
       </c>
@@ -3383,8 +3617,12 @@
       <c r="V42" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W42" s="6"/>
+      <c r="X42" s="6"/>
+      <c r="Y42" s="6"/>
+      <c r="Z42" s="6"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
@@ -3447,8 +3685,12 @@
       <c r="V43" s="16" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W43" s="6"/>
+      <c r="X43" s="6"/>
+      <c r="Y43" s="6"/>
+      <c r="Z43" s="6"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>72</v>
       </c>
@@ -3511,8 +3753,12 @@
       <c r="V44" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W44" s="6"/>
+      <c r="X44" s="6"/>
+      <c r="Y44" s="6"/>
+      <c r="Z44" s="6"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>73</v>
       </c>
@@ -3575,8 +3821,12 @@
       <c r="V45" s="16" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W45" s="6"/>
+      <c r="X45" s="6"/>
+      <c r="Y45" s="6"/>
+      <c r="Z45" s="6"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>73</v>
       </c>
@@ -3639,8 +3889,12 @@
       <c r="V46" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W46" s="6"/>
+      <c r="X46" s="6"/>
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>73</v>
       </c>
@@ -3703,8 +3957,12 @@
       <c r="V47" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W47" s="6"/>
+      <c r="X47" s="6"/>
+      <c r="Y47" s="6"/>
+      <c r="Z47" s="6"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>73</v>
       </c>
@@ -3767,8 +4025,12 @@
       <c r="V48" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W48" s="6"/>
+      <c r="X48" s="6"/>
+      <c r="Y48" s="6"/>
+      <c r="Z48" s="6"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>72</v>
       </c>
@@ -3831,8 +4093,12 @@
       <c r="V49" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W49" s="6"/>
+      <c r="X49" s="6"/>
+      <c r="Y49" s="6"/>
+      <c r="Z49" s="6"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>73</v>
       </c>
@@ -3889,8 +4155,12 @@
       <c r="V50" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W50" s="6"/>
+      <c r="X50" s="6"/>
+      <c r="Y50" s="6"/>
+      <c r="Z50" s="6"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>73</v>
       </c>
@@ -3935,8 +4205,12 @@
       <c r="T51" s="6"/>
       <c r="U51" s="6"/>
       <c r="V51" s="6"/>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W51" s="6"/>
+      <c r="X51" s="6"/>
+      <c r="Y51" s="6"/>
+      <c r="Z51" s="6"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>73</v>
       </c>
@@ -3999,8 +4273,12 @@
       <c r="V52" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W52" s="6"/>
+      <c r="X52" s="6"/>
+      <c r="Y52" s="6"/>
+      <c r="Z52" s="6"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>73</v>
       </c>
@@ -4063,8 +4341,12 @@
       <c r="V53" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W53" s="6"/>
+      <c r="X53" s="6"/>
+      <c r="Y53" s="6"/>
+      <c r="Z53" s="6"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>73</v>
       </c>
@@ -4109,8 +4391,12 @@
       <c r="T54" s="6"/>
       <c r="U54" s="6"/>
       <c r="V54" s="6"/>
-    </row>
-    <row r="55" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W54" s="6"/>
+      <c r="X54" s="6"/>
+      <c r="Y54" s="6"/>
+      <c r="Z54" s="6"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>73</v>
       </c>
@@ -4155,8 +4441,12 @@
       <c r="T55" s="6"/>
       <c r="U55" s="6"/>
       <c r="V55" s="6"/>
-    </row>
-    <row r="56" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W55" s="6"/>
+      <c r="X55" s="6"/>
+      <c r="Y55" s="6"/>
+      <c r="Z55" s="6"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>73</v>
       </c>
@@ -4201,8 +4491,12 @@
       <c r="T56" s="6"/>
       <c r="U56" s="6"/>
       <c r="V56" s="6"/>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W56" s="6"/>
+      <c r="X56" s="6"/>
+      <c r="Y56" s="6"/>
+      <c r="Z56" s="6"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>73</v>
       </c>
@@ -4265,8 +4559,12 @@
       <c r="V57" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W57" s="6"/>
+      <c r="X57" s="6"/>
+      <c r="Y57" s="6"/>
+      <c r="Z57" s="6"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>73</v>
       </c>
@@ -4329,8 +4627,12 @@
       <c r="V58" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="59" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W58" s="6"/>
+      <c r="X58" s="6"/>
+      <c r="Y58" s="6"/>
+      <c r="Z58" s="6"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>73</v>
       </c>
@@ -4375,8 +4677,12 @@
       <c r="T59" s="6"/>
       <c r="U59" s="6"/>
       <c r="V59" s="6"/>
-    </row>
-    <row r="60" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W59" s="6"/>
+      <c r="X59" s="6"/>
+      <c r="Y59" s="6"/>
+      <c r="Z59" s="6"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>73</v>
       </c>
@@ -4421,8 +4727,12 @@
       <c r="T60" s="6"/>
       <c r="U60" s="6"/>
       <c r="V60" s="6"/>
-    </row>
-    <row r="61" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W60" s="6"/>
+      <c r="X60" s="6"/>
+      <c r="Y60" s="6"/>
+      <c r="Z60" s="6"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>73</v>
       </c>
@@ -4467,8 +4777,12 @@
       <c r="T61" s="6"/>
       <c r="U61" s="6"/>
       <c r="V61" s="6"/>
-    </row>
-    <row r="62" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W61" s="6"/>
+      <c r="X61" s="6"/>
+      <c r="Y61" s="6"/>
+      <c r="Z61" s="6"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>73</v>
       </c>
@@ -4513,8 +4827,12 @@
       <c r="T62" s="6"/>
       <c r="U62" s="6"/>
       <c r="V62" s="6"/>
-    </row>
-    <row r="63" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W62" s="6"/>
+      <c r="X62" s="6"/>
+      <c r="Y62" s="6"/>
+      <c r="Z62" s="6"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>73</v>
       </c>
@@ -4559,8 +4877,12 @@
       <c r="T63" s="6"/>
       <c r="U63" s="6"/>
       <c r="V63" s="6"/>
-    </row>
-    <row r="64" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W63" s="6"/>
+      <c r="X63" s="6"/>
+      <c r="Y63" s="6"/>
+      <c r="Z63" s="6"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>73</v>
       </c>
@@ -4605,8 +4927,12 @@
       <c r="T64" s="6"/>
       <c r="U64" s="6"/>
       <c r="V64" s="6"/>
-    </row>
-    <row r="65" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W64" s="6"/>
+      <c r="X64" s="6"/>
+      <c r="Y64" s="6"/>
+      <c r="Z64" s="6"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>73</v>
       </c>
@@ -4651,8 +4977,12 @@
       <c r="T65" s="6"/>
       <c r="U65" s="6"/>
       <c r="V65" s="6"/>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W65" s="6"/>
+      <c r="X65" s="6"/>
+      <c r="Y65" s="6"/>
+      <c r="Z65" s="6"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4" t="s">
@@ -4677,6 +5007,56 @@
       <c r="T66" s="6"/>
       <c r="U66" s="6"/>
       <c r="V66" s="6"/>
+      <c r="W66" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="X66" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y66" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z66" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="6"/>
+      <c r="S67" s="6"/>
+      <c r="T67" s="6"/>
+      <c r="U67" s="6"/>
+      <c r="V67" s="6"/>
+      <c r="W67" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="X67" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y67" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z67" s="6" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>